<commit_message>
Config File Updates 4/23/24
Audio Visual renamed to Audio Visual Services, new Administrative request type - Work related injury or illness
</commit_message>
<xml_diff>
--- a/helpUtils/umbchelp_reqtype_config.xlsx
+++ b/helpUtils/umbchelp_reqtype_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kensch\Box\RT-Root\RT-Folders\RT-Config-and-Form-Data\NEW myUMBC Support-RT-Dev-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kensch\Box\10. Enterprise Applications\RT-Root\RT-Folders\RT-Config-and-Form-Data\NEW myUMBC Support-RT-Dev-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73687092-20E6-4782-B683-6720481018D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3301AF-6A22-4C4C-B695-DCFAC4227D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25170" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="645" windowWidth="19350" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="studentfaculty_reqtype_config" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="454">
   <si>
     <t>Service Area</t>
   </si>
@@ -584,9 +584,6 @@
     <t>Special Collections</t>
   </si>
   <si>
-    <t>The Special Collections department collects materials of enduring historical and cultural value—housing, preserving, and making accessible materials that are original, rare, unique, fragile, and archival. Our collections and staff support UMBC’s research and educational mission and its dedication to cultural and ethnic diversity, social responsibility, and lifelong learning.</t>
-  </si>
-  <si>
     <t>https://library.umbc.edu/specialcollections/</t>
   </si>
   <si>
@@ -1498,6 +1495,22 @@
   </si>
   <si>
     <t>webdevelopmentTags</t>
+  </si>
+  <si>
+    <t>The Special Collections department collects materials of enduring historical and cultural value—housing, preserving, and making accessible materials that are original, rare, unique, fragile, and archival. Our collections and staff support UMBC’s research and educational mission and its dedication to cultural and ethnic diversity, social responsibility, and lifelong learning.
+We offer on-site services in addition to remote support to all researchers. For assistance with research, accessing collection materials, or preparing instruction, please contact the Special Collections staff directly at speccoll@umbc.edu.</t>
+  </si>
+  <si>
+    <t>Work Related Injury or Illness</t>
+  </si>
+  <si>
+    <t>https://safety.umbc.edu/work-related-injury-or-illness/</t>
+  </si>
+  <si>
+    <t>eshTags</t>
+  </si>
+  <si>
+    <t>All work related injuries should be addressed as soon as possible. Use the guidance at the linked Request Help page to properly report and seek treatment for your injury.</t>
   </si>
 </sst>
 </file>
@@ -2044,7 +2057,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2056,6 +2069,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2414,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3332,7 +3348,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" ht="141.75">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -3342,23 +3358,23 @@
       <c r="C32" t="s">
         <v>152</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
         <v>153</v>
       </c>
-      <c r="E32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" t="s">
         <v>154</v>
-      </c>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3366,13 +3382,13 @@
         <v>9</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" t="s">
         <v>156</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>157</v>
-      </c>
-      <c r="D33" t="s">
-        <v>158</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -3381,13 +3397,13 @@
         <v>32</v>
       </c>
       <c r="G33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" t="s">
         <v>159</v>
-      </c>
-      <c r="H33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3395,13 +3411,13 @@
         <v>9</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" t="s">
         <v>161</v>
-      </c>
-      <c r="D34" t="s">
-        <v>162</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -3410,13 +3426,13 @@
         <v>32</v>
       </c>
       <c r="G34" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
         <v>163</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3424,13 +3440,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" t="s">
         <v>165</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>166</v>
-      </c>
-      <c r="D35" t="s">
-        <v>167</v>
       </c>
       <c r="E35" t="s">
         <v>26</v>
@@ -3439,13 +3455,13 @@
         <v>20</v>
       </c>
       <c r="G35" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" t="s">
         <v>168</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>169</v>
-      </c>
-      <c r="I35" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3453,13 +3469,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E36" t="s">
         <v>26</v>
@@ -3468,13 +3484,13 @@
         <v>20</v>
       </c>
       <c r="G36" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" t="s">
         <v>172</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>173</v>
-      </c>
-      <c r="I36" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3482,13 +3498,13 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C37" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" t="s">
         <v>175</v>
-      </c>
-      <c r="D37" t="s">
-        <v>176</v>
       </c>
       <c r="E37" t="s">
         <v>26</v>
@@ -3497,13 +3513,13 @@
         <v>20</v>
       </c>
       <c r="G37" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" t="s">
         <v>177</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>178</v>
-      </c>
-      <c r="I37" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3511,13 +3527,13 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" t="s">
         <v>180</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -3526,13 +3542,13 @@
         <v>32</v>
       </c>
       <c r="G38" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
         <v>183</v>
-      </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -3540,13 +3556,13 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -3555,13 +3571,13 @@
         <v>32</v>
       </c>
       <c r="G39" t="s">
+        <v>186</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
         <v>187</v>
-      </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3569,28 +3585,28 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" t="s">
         <v>189</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" t="s">
         <v>190</v>
       </c>
-      <c r="E40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
         <v>191</v>
-      </c>
-      <c r="H40" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3598,13 +3614,13 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -3613,13 +3629,13 @@
         <v>32</v>
       </c>
       <c r="G41" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" t="s">
         <v>195</v>
-      </c>
-      <c r="H41" t="s">
-        <v>15</v>
-      </c>
-      <c r="I41" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3627,13 +3643,13 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C42" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -3642,13 +3658,13 @@
         <v>32</v>
       </c>
       <c r="G42" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" t="s">
         <v>199</v>
-      </c>
-      <c r="H42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3656,13 +3672,13 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
+        <v>200</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -3671,13 +3687,13 @@
         <v>32</v>
       </c>
       <c r="G43" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s">
         <v>203</v>
-      </c>
-      <c r="H43" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3685,13 +3701,13 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C44" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -3700,13 +3716,13 @@
         <v>32</v>
       </c>
       <c r="G44" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
         <v>207</v>
-      </c>
-      <c r="H44" t="s">
-        <v>15</v>
-      </c>
-      <c r="I44" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3714,28 +3730,28 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" t="s">
         <v>209</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" t="s">
         <v>210</v>
       </c>
-      <c r="E45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
         <v>211</v>
-      </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3743,13 +3759,13 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" t="s">
         <v>213</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>214</v>
-      </c>
-      <c r="D46" t="s">
-        <v>215</v>
       </c>
       <c r="E46" t="s">
         <v>26</v>
@@ -3761,18 +3777,18 @@
         <v>15</v>
       </c>
       <c r="H46" t="s">
+        <v>215</v>
+      </c>
+      <c r="I46" t="s">
         <v>216</v>
-      </c>
-      <c r="I46" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
         <v>68</v>
@@ -3798,16 +3814,16 @@
     </row>
     <row r="48" spans="1:9" ht="126">
       <c r="A48" t="s">
+        <v>217</v>
+      </c>
+      <c r="B48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" t="s">
         <v>218</v>
       </c>
-      <c r="B48" t="s">
-        <v>185</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D48" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -3816,27 +3832,27 @@
         <v>32</v>
       </c>
       <c r="G48" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
         <v>221</v>
-      </c>
-      <c r="H48" t="s">
-        <v>15</v>
-      </c>
-      <c r="I48" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C49" t="s">
+        <v>222</v>
+      </c>
+      <c r="D49" t="s">
         <v>223</v>
-      </c>
-      <c r="D49" t="s">
-        <v>224</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -3845,27 +3861,27 @@
         <v>32</v>
       </c>
       <c r="G49" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
         <v>225</v>
-      </c>
-      <c r="H49" t="s">
-        <v>15</v>
-      </c>
-      <c r="I49" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C50" t="s">
         <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
@@ -3885,16 +3901,16 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D51" t="s">
         <v>228</v>
-      </c>
-      <c r="D51" t="s">
-        <v>229</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
@@ -3903,65 +3919,65 @@
         <v>32</v>
       </c>
       <c r="G51" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
         <v>230</v>
-      </c>
-      <c r="H51" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B52" t="s">
+        <v>231</v>
+      </c>
+      <c r="C52" t="s">
         <v>232</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>233</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" t="s">
         <v>234</v>
       </c>
-      <c r="E52" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" t="s">
         <v>235</v>
-      </c>
-      <c r="H52" t="s">
-        <v>15</v>
-      </c>
-      <c r="I52" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B53" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" t="s">
         <v>237</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>238</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" t="s">
         <v>239</v>
-      </c>
-      <c r="E53" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" t="s">
-        <v>240</v>
       </c>
       <c r="H53" t="s">
         <v>15</v>
@@ -3972,45 +3988,45 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C54" t="s">
+        <v>240</v>
+      </c>
+      <c r="D54" t="s">
         <v>241</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" t="s">
         <v>242</v>
       </c>
-      <c r="E54" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
         <v>243</v>
-      </c>
-      <c r="H54" t="s">
-        <v>15</v>
-      </c>
-      <c r="I54" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B55" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C55" t="s">
+        <v>244</v>
+      </c>
+      <c r="D55" t="s">
         <v>245</v>
-      </c>
-      <c r="D55" t="s">
-        <v>246</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -4019,44 +4035,44 @@
         <v>32</v>
       </c>
       <c r="G55" t="s">
+        <v>246</v>
+      </c>
+      <c r="I55" t="s">
         <v>247</v>
-      </c>
-      <c r="I55" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C56" t="s">
+        <v>248</v>
+      </c>
+      <c r="D56" t="s">
         <v>249</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56" t="s">
         <v>250</v>
       </c>
-      <c r="E56" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" t="s">
         <v>251</v>
-      </c>
-      <c r="H56" t="s">
-        <v>15</v>
-      </c>
-      <c r="I56" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B57" t="s">
         <v>106</v>
@@ -4085,16 +4101,16 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B58" t="s">
         <v>106</v>
       </c>
       <c r="C58" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -4103,27 +4119,27 @@
         <v>32</v>
       </c>
       <c r="G58" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
         <v>195</v>
-      </c>
-      <c r="H58" t="s">
-        <v>15</v>
-      </c>
-      <c r="I58" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B59" t="s">
         <v>106</v>
       </c>
       <c r="C59" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -4132,85 +4148,85 @@
         <v>32</v>
       </c>
       <c r="G59" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
         <v>207</v>
-      </c>
-      <c r="H59" t="s">
-        <v>15</v>
-      </c>
-      <c r="I59" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B60" t="s">
-        <v>253</v>
+        <v>106</v>
       </c>
       <c r="C60" t="s">
-        <v>254</v>
-      </c>
-      <c r="D60" t="s">
-        <v>255</v>
+        <v>450</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="E60" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F60" t="s">
         <v>32</v>
       </c>
-      <c r="G60" t="s">
-        <v>256</v>
+      <c r="G60" s="5" t="s">
+        <v>451</v>
       </c>
       <c r="H60" t="s">
         <v>15</v>
       </c>
       <c r="I60" t="s">
-        <v>257</v>
+        <v>452</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>218</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>156</v>
+        <v>217</v>
+      </c>
+      <c r="B61" t="s">
+        <v>252</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>253</v>
       </c>
       <c r="D61" t="s">
-        <v>158</v>
+        <v>254</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F61" t="s">
         <v>32</v>
       </c>
       <c r="G61" t="s">
-        <v>159</v>
+        <v>255</v>
       </c>
       <c r="H61" t="s">
         <v>15</v>
       </c>
       <c r="I61" t="s">
-        <v>160</v>
+        <v>256</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" t="s">
         <v>156</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D62" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -4218,28 +4234,28 @@
       <c r="F62" t="s">
         <v>32</v>
       </c>
-      <c r="G62" s="5" t="s">
-        <v>163</v>
+      <c r="G62" t="s">
+        <v>158</v>
       </c>
       <c r="H62" t="s">
         <v>15</v>
       </c>
       <c r="I62" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>218</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C63" t="s">
-        <v>259</v>
+        <v>217</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="D63" t="s">
-        <v>260</v>
+        <v>161</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -4247,28 +4263,28 @@
       <c r="F63" t="s">
         <v>32</v>
       </c>
-      <c r="G63" t="s">
-        <v>261</v>
+      <c r="G63" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="H63" t="s">
         <v>15</v>
       </c>
       <c r="I63" t="s">
-        <v>262</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C64" t="s">
-        <v>264</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
+      </c>
+      <c r="D64" t="s">
+        <v>259</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -4276,28 +4292,28 @@
       <c r="F64" t="s">
         <v>32</v>
       </c>
-      <c r="G64" s="5" t="s">
-        <v>266</v>
+      <c r="G64" t="s">
+        <v>260</v>
       </c>
       <c r="H64" t="s">
         <v>15</v>
       </c>
       <c r="I64" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" t="s">
         <v>263</v>
       </c>
-      <c r="C65" t="s">
-        <v>268</v>
-      </c>
-      <c r="D65" t="s">
-        <v>269</v>
+      <c r="D65" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -4306,27 +4322,27 @@
         <v>32</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H65" t="s">
         <v>15</v>
       </c>
       <c r="I65" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D66" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -4335,27 +4351,27 @@
         <v>32</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H66" t="s">
         <v>15</v>
       </c>
       <c r="I66" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C67" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D67" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -4364,27 +4380,27 @@
         <v>32</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H67" t="s">
         <v>15</v>
       </c>
       <c r="I67" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C68" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D68" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -4393,24 +4409,27 @@
         <v>32</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H68" t="s">
         <v>15</v>
       </c>
       <c r="I68" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C69" t="s">
-        <v>284</v>
+        <v>279</v>
+      </c>
+      <c r="D69" t="s">
+        <v>280</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -4419,56 +4438,53 @@
         <v>32</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H69" t="s">
         <v>15</v>
       </c>
       <c r="I69" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>218</v>
-      </c>
-      <c r="B70" t="s">
-        <v>287</v>
+        <v>217</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="C70" t="s">
-        <v>288</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F70" t="s">
         <v>32</v>
       </c>
-      <c r="G70" t="s">
-        <v>290</v>
+      <c r="G70" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="H70" t="s">
         <v>15</v>
       </c>
       <c r="I70" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B71" t="s">
+        <v>286</v>
+      </c>
+      <c r="C71" t="s">
         <v>287</v>
       </c>
-      <c r="C71" t="s">
-        <v>292</v>
-      </c>
       <c r="D71" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E71" t="s">
         <v>26</v>
@@ -4477,27 +4493,27 @@
         <v>32</v>
       </c>
       <c r="G71" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H71" t="s">
         <v>15</v>
       </c>
       <c r="I71" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C72" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E72" t="s">
         <v>26</v>
@@ -4505,28 +4521,28 @@
       <c r="F72" t="s">
         <v>32</v>
       </c>
-      <c r="G72" s="5" t="s">
-        <v>298</v>
+      <c r="G72" t="s">
+        <v>293</v>
       </c>
       <c r="H72" t="s">
         <v>15</v>
       </c>
       <c r="I72" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B73" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C73" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E73" t="s">
         <v>26</v>
@@ -4534,28 +4550,28 @@
       <c r="F73" t="s">
         <v>32</v>
       </c>
-      <c r="G73" t="s">
-        <v>302</v>
+      <c r="G73" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="H73" t="s">
         <v>15</v>
       </c>
       <c r="I73" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B74" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C74" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E74" t="s">
         <v>26</v>
@@ -4564,27 +4580,27 @@
         <v>32</v>
       </c>
       <c r="G74" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H74" t="s">
         <v>15</v>
       </c>
       <c r="I74" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B75" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C75" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E75" t="s">
         <v>26</v>
@@ -4593,27 +4609,27 @@
         <v>32</v>
       </c>
       <c r="G75" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H75" t="s">
         <v>15</v>
       </c>
       <c r="I75" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C76" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E76" t="s">
         <v>26</v>
@@ -4621,28 +4637,28 @@
       <c r="F76" t="s">
         <v>32</v>
       </c>
-      <c r="G76" s="5" t="s">
-        <v>314</v>
+      <c r="G76" t="s">
+        <v>309</v>
       </c>
       <c r="H76" t="s">
         <v>15</v>
       </c>
       <c r="I76" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C77" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E77" t="s">
         <v>26</v>
@@ -4651,27 +4667,27 @@
         <v>32</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H77" t="s">
         <v>15</v>
       </c>
       <c r="I77" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C78" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E78" t="s">
         <v>26</v>
@@ -4680,27 +4696,27 @@
         <v>32</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H78" t="s">
         <v>15</v>
       </c>
       <c r="I78" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B79" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C79" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E79" t="s">
         <v>26</v>
@@ -4709,114 +4725,114 @@
         <v>32</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H79" t="s">
         <v>15</v>
       </c>
       <c r="I79" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="C80" t="s">
-        <v>214</v>
-      </c>
-      <c r="D80" t="s">
-        <v>215</v>
+        <v>323</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="E80" t="s">
         <v>26</v>
       </c>
       <c r="F80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>325</v>
       </c>
       <c r="H80" t="s">
-        <v>216</v>
+        <v>15</v>
       </c>
       <c r="I80" t="s">
-        <v>217</v>
+        <v>326</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>328</v>
+        <v>217</v>
       </c>
       <c r="B81" t="s">
-        <v>329</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>330</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>331</v>
+        <v>213</v>
+      </c>
+      <c r="D81" t="s">
+        <v>214</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G81" t="s">
-        <v>332</v>
+        <v>15</v>
       </c>
       <c r="H81" t="s">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="I81" t="s">
-        <v>333</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
+        <v>327</v>
+      </c>
+      <c r="B82" t="s">
         <v>328</v>
       </c>
-      <c r="B82" t="s">
-        <v>334</v>
-      </c>
       <c r="C82" t="s">
-        <v>335</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>336</v>
+        <v>329</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="E82" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F82" t="s">
         <v>32</v>
       </c>
       <c r="G82" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="H82" t="s">
         <v>15</v>
       </c>
       <c r="I82" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B83" t="s">
+        <v>333</v>
+      </c>
+      <c r="C83" t="s">
         <v>334</v>
       </c>
-      <c r="C83" t="s">
-        <v>339</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>340</v>
+      <c r="D83" s="6" t="s">
+        <v>335</v>
       </c>
       <c r="E83" t="s">
         <v>26</v>
@@ -4825,27 +4841,27 @@
         <v>32</v>
       </c>
       <c r="G83" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H83" t="s">
         <v>15</v>
       </c>
       <c r="I83" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B84" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C84" t="s">
-        <v>343</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>344</v>
+        <v>338</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="E84" t="s">
         <v>26</v>
@@ -4854,27 +4870,27 @@
         <v>32</v>
       </c>
       <c r="G84" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H84" t="s">
         <v>15</v>
       </c>
       <c r="I84" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B85" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C85" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E85" t="s">
         <v>26</v>
@@ -4883,27 +4899,27 @@
         <v>32</v>
       </c>
       <c r="G85" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="H85" t="s">
         <v>15</v>
       </c>
       <c r="I85" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B86" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C86" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E86" t="s">
         <v>26</v>
@@ -4912,27 +4928,27 @@
         <v>32</v>
       </c>
       <c r="G86" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="H86" t="s">
         <v>15</v>
       </c>
       <c r="I86" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B87" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C87" t="s">
-        <v>355</v>
-      </c>
-      <c r="D87" t="s">
-        <v>356</v>
+        <v>350</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>351</v>
       </c>
       <c r="E87" t="s">
         <v>26</v>
@@ -4941,27 +4957,27 @@
         <v>32</v>
       </c>
       <c r="G87" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="H87" t="s">
         <v>15</v>
       </c>
       <c r="I87" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B88" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C88" t="s">
-        <v>359</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>360</v>
+        <v>354</v>
+      </c>
+      <c r="D88" t="s">
+        <v>355</v>
       </c>
       <c r="E88" t="s">
         <v>26</v>
@@ -4970,27 +4986,27 @@
         <v>32</v>
       </c>
       <c r="G88" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H88" t="s">
         <v>15</v>
       </c>
       <c r="I88" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>328</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>363</v>
+        <v>327</v>
+      </c>
+      <c r="B89" t="s">
+        <v>333</v>
       </c>
       <c r="C89" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E89" t="s">
         <v>26</v>
@@ -4999,27 +5015,27 @@
         <v>32</v>
       </c>
       <c r="G89" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H89" t="s">
         <v>15</v>
       </c>
       <c r="I89" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C90" t="s">
         <v>363</v>
       </c>
-      <c r="C90" t="s">
-        <v>368</v>
-      </c>
       <c r="D90" s="6" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E90" t="s">
         <v>26</v>
@@ -5028,27 +5044,27 @@
         <v>32</v>
       </c>
       <c r="G90" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H90" t="s">
         <v>15</v>
       </c>
       <c r="I90" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C91" t="s">
-        <v>343</v>
+        <v>367</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>344</v>
+        <v>368</v>
       </c>
       <c r="E91" t="s">
         <v>26</v>
@@ -5057,114 +5073,114 @@
         <v>32</v>
       </c>
       <c r="G91" t="s">
-        <v>345</v>
+        <v>369</v>
       </c>
       <c r="H91" t="s">
         <v>15</v>
       </c>
       <c r="I91" t="s">
-        <v>346</v>
+        <v>370</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C92" t="s">
+        <v>342</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="E92" t="s">
+        <v>26</v>
+      </c>
+      <c r="F92" t="s">
+        <v>32</v>
+      </c>
+      <c r="G92" t="s">
+        <v>344</v>
+      </c>
+      <c r="H92" t="s">
+        <v>15</v>
+      </c>
+      <c r="I92" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" t="s">
+        <v>327</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C93" t="s">
+        <v>371</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="E93" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" t="s">
+        <v>32</v>
+      </c>
+      <c r="G93" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="E92" t="s">
-        <v>26</v>
-      </c>
-      <c r="F92" t="s">
-        <v>32</v>
-      </c>
-      <c r="G92" s="5" t="s">
+      <c r="H93" t="s">
+        <v>15</v>
+      </c>
+      <c r="I93" t="s">
         <v>374</v>
       </c>
-      <c r="H92" t="s">
-        <v>15</v>
-      </c>
-      <c r="I92" t="s">
+    </row>
+    <row r="94" spans="1:9" ht="78.75">
+      <c r="A94" t="s">
+        <v>327</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="78.75">
-      <c r="A93" t="s">
-        <v>328</v>
-      </c>
-      <c r="B93" s="2" t="s">
+      <c r="C94" t="s">
         <v>376</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D94" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="D93" s="10" t="s">
+      <c r="E94" t="s">
+        <v>26</v>
+      </c>
+      <c r="F94" t="s">
+        <v>32</v>
+      </c>
+      <c r="G94" t="s">
         <v>378</v>
       </c>
-      <c r="E93" t="s">
-        <v>26</v>
-      </c>
-      <c r="F93" t="s">
-        <v>32</v>
-      </c>
-      <c r="G93" t="s">
+      <c r="H94" t="s">
+        <v>15</v>
+      </c>
+      <c r="I94" t="s">
         <v>379</v>
-      </c>
-      <c r="H93" t="s">
-        <v>15</v>
-      </c>
-      <c r="I93" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" t="s">
-        <v>328</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C94" t="s">
-        <v>381</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="E94" t="s">
-        <v>26</v>
-      </c>
-      <c r="F94" t="s">
-        <v>32</v>
-      </c>
-      <c r="G94" t="s">
-        <v>383</v>
-      </c>
-      <c r="H94" t="s">
-        <v>15</v>
-      </c>
-      <c r="I94" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C95" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E95" t="s">
         <v>26</v>
@@ -5173,27 +5189,27 @@
         <v>32</v>
       </c>
       <c r="G95" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H95" t="s">
         <v>15</v>
       </c>
       <c r="I95" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C96" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E96" t="s">
         <v>26</v>
@@ -5202,27 +5218,27 @@
         <v>32</v>
       </c>
       <c r="G96" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="H96" t="s">
         <v>15</v>
       </c>
       <c r="I96" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C97" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E97" t="s">
         <v>26</v>
@@ -5231,27 +5247,27 @@
         <v>32</v>
       </c>
       <c r="G97" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="H97" t="s">
         <v>15</v>
       </c>
       <c r="I97" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C98" t="s">
-        <v>397</v>
-      </c>
-      <c r="D98" t="s">
-        <v>398</v>
+        <v>392</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>393</v>
       </c>
       <c r="E98" t="s">
         <v>26</v>
@@ -5260,27 +5276,27 @@
         <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="H98" t="s">
         <v>15</v>
       </c>
       <c r="I98" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="C99" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D99" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E99" t="s">
         <v>26</v>
@@ -5289,27 +5305,27 @@
         <v>32</v>
       </c>
       <c r="G99" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H99" t="s">
         <v>15</v>
       </c>
       <c r="I99" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C100" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D100" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E100" t="s">
         <v>26</v>
@@ -5318,56 +5334,56 @@
         <v>32</v>
       </c>
       <c r="G100" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="H100" t="s">
         <v>15</v>
       </c>
       <c r="I100" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C101" t="s">
+        <v>405</v>
+      </c>
+      <c r="D101" t="s">
         <v>406</v>
       </c>
-      <c r="C101" t="s">
-        <v>410</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>411</v>
-      </c>
       <c r="E101" t="s">
         <v>26</v>
       </c>
       <c r="F101" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G101" t="s">
-        <v>15</v>
+        <v>407</v>
       </c>
       <c r="H101" t="s">
-        <v>412</v>
+        <v>15</v>
       </c>
       <c r="I101" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C102" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E102" t="s">
         <v>26</v>
@@ -5379,53 +5395,53 @@
         <v>15</v>
       </c>
       <c r="H102" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="I102" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="C103" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="E103" t="s">
         <v>26</v>
       </c>
       <c r="F103" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G103" t="s">
-        <v>421</v>
+        <v>15</v>
       </c>
       <c r="H103" t="s">
-        <v>15</v>
+        <v>415</v>
       </c>
       <c r="I103" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>328</v>
-      </c>
-      <c r="B104" t="s">
+        <v>327</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C104" t="s">
         <v>418</v>
       </c>
-      <c r="C104" t="s">
-        <v>423</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>424</v>
+      <c r="D104" s="6" t="s">
+        <v>419</v>
       </c>
       <c r="E104" t="s">
         <v>26</v>
@@ -5434,27 +5450,27 @@
         <v>32</v>
       </c>
       <c r="G104" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="H104" t="s">
         <v>15</v>
       </c>
       <c r="I104" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>328</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>418</v>
+        <v>327</v>
+      </c>
+      <c r="B105" t="s">
+        <v>417</v>
       </c>
       <c r="C105" t="s">
-        <v>377</v>
-      </c>
-      <c r="D105" t="s">
-        <v>378</v>
+        <v>422</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>423</v>
       </c>
       <c r="E105" t="s">
         <v>26</v>
@@ -5463,27 +5479,27 @@
         <v>32</v>
       </c>
       <c r="G105" t="s">
-        <v>379</v>
+        <v>424</v>
       </c>
       <c r="H105" t="s">
         <v>15</v>
       </c>
       <c r="I105" t="s">
-        <v>380</v>
+        <v>425</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>328</v>
-      </c>
-      <c r="B106" t="s">
-        <v>418</v>
+        <v>327</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="C106" t="s">
-        <v>427</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>428</v>
+        <v>376</v>
+      </c>
+      <c r="D106" t="s">
+        <v>377</v>
       </c>
       <c r="E106" t="s">
         <v>26</v>
@@ -5491,28 +5507,28 @@
       <c r="F106" t="s">
         <v>32</v>
       </c>
-      <c r="G106" s="5" t="s">
-        <v>429</v>
+      <c r="G106" t="s">
+        <v>378</v>
       </c>
       <c r="H106" t="s">
         <v>15</v>
       </c>
       <c r="I106" t="s">
-        <v>430</v>
+        <v>379</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B107" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C107" t="s">
-        <v>431</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>432</v>
+        <v>426</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>427</v>
       </c>
       <c r="E107" t="s">
         <v>26</v>
@@ -5520,28 +5536,28 @@
       <c r="F107" t="s">
         <v>32</v>
       </c>
-      <c r="G107" t="s">
-        <v>433</v>
+      <c r="G107" s="5" t="s">
+        <v>428</v>
       </c>
       <c r="H107" t="s">
         <v>15</v>
       </c>
       <c r="I107" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B108" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C108" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E108" t="s">
         <v>26</v>
@@ -5550,27 +5566,27 @@
         <v>32</v>
       </c>
       <c r="G108" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="H108" t="s">
         <v>15</v>
       </c>
       <c r="I108" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B109" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C109" t="s">
-        <v>397</v>
-      </c>
-      <c r="D109" t="s">
-        <v>398</v>
+        <v>434</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>435</v>
       </c>
       <c r="E109" t="s">
         <v>26</v>
@@ -5579,27 +5595,27 @@
         <v>32</v>
       </c>
       <c r="G109" t="s">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="H109" t="s">
         <v>15</v>
       </c>
       <c r="I109" t="s">
-        <v>400</v>
+        <v>436</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B110" t="s">
-        <v>418</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>439</v>
+        <v>417</v>
+      </c>
+      <c r="C110" t="s">
+        <v>396</v>
+      </c>
+      <c r="D110" t="s">
+        <v>397</v>
       </c>
       <c r="E110" t="s">
         <v>26</v>
@@ -5608,27 +5624,27 @@
         <v>32</v>
       </c>
       <c r="G110" t="s">
-        <v>440</v>
+        <v>398</v>
       </c>
       <c r="H110" t="s">
         <v>15</v>
       </c>
       <c r="I110" t="s">
-        <v>441</v>
+        <v>399</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B111" t="s">
-        <v>442</v>
-      </c>
-      <c r="C111" t="s">
-        <v>443</v>
-      </c>
-      <c r="D111" t="s">
-        <v>444</v>
+        <v>417</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>438</v>
       </c>
       <c r="E111" t="s">
         <v>26</v>
@@ -5637,27 +5653,27 @@
         <v>32</v>
       </c>
       <c r="G111" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H111" t="s">
         <v>15</v>
       </c>
       <c r="I111" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B112" t="s">
+        <v>441</v>
+      </c>
+      <c r="C112" t="s">
         <v>442</v>
       </c>
-      <c r="C112" t="s">
-        <v>343</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>344</v>
+      <c r="D112" t="s">
+        <v>443</v>
       </c>
       <c r="E112" t="s">
         <v>26</v>
@@ -5666,27 +5682,27 @@
         <v>32</v>
       </c>
       <c r="G112" t="s">
-        <v>345</v>
+        <v>444</v>
       </c>
       <c r="H112" t="s">
         <v>15</v>
       </c>
       <c r="I112" t="s">
-        <v>346</v>
+        <v>445</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B113" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C113" t="s">
-        <v>442</v>
+        <v>342</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>447</v>
+        <v>343</v>
       </c>
       <c r="E113" t="s">
         <v>26</v>
@@ -5695,63 +5711,92 @@
         <v>32</v>
       </c>
       <c r="G113" t="s">
-        <v>448</v>
+        <v>344</v>
       </c>
       <c r="H113" t="s">
         <v>15</v>
       </c>
       <c r="I113" t="s">
-        <v>449</v>
+        <v>345</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B114" t="s">
+        <v>441</v>
+      </c>
+      <c r="C114" t="s">
+        <v>441</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E114" t="s">
+        <v>26</v>
+      </c>
+      <c r="F114" t="s">
+        <v>32</v>
+      </c>
+      <c r="G114" t="s">
+        <v>447</v>
+      </c>
+      <c r="H114" t="s">
+        <v>15</v>
+      </c>
+      <c r="I114" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>327</v>
+      </c>
+      <c r="B115" t="s">
+        <v>212</v>
+      </c>
+      <c r="C115" t="s">
         <v>213</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D115" t="s">
         <v>214</v>
       </c>
-      <c r="D114" t="s">
+      <c r="E115" t="s">
+        <v>26</v>
+      </c>
+      <c r="F115" t="s">
+        <v>14</v>
+      </c>
+      <c r="G115" t="s">
+        <v>15</v>
+      </c>
+      <c r="H115" t="s">
         <v>215</v>
       </c>
-      <c r="E114" t="s">
-        <v>26</v>
-      </c>
-      <c r="F114" t="s">
-        <v>14</v>
-      </c>
-      <c r="G114" t="s">
-        <v>15</v>
-      </c>
-      <c r="H114" t="s">
+      <c r="I115" t="s">
         <v>216</v>
       </c>
-      <c r="I114" t="s">
-        <v>217</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I114">
-    <sortCondition ref="B4:B114"/>
-    <sortCondition ref="C4:C114"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I115">
+    <sortCondition ref="B4:B115"/>
+    <sortCondition ref="C4:C115"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G72" r:id="rId1" xr:uid="{0A8B3BE8-26AA-754F-BFC2-92BCE65A3ED5}"/>
-    <hyperlink ref="G76" r:id="rId2" xr:uid="{3651323E-D02C-0B41-ADBD-75C73D14B3F2}"/>
-    <hyperlink ref="G78" r:id="rId3" xr:uid="{13893242-B741-7745-BC62-72A5ABF3FA62}"/>
-    <hyperlink ref="G79" r:id="rId4" xr:uid="{2960CE5E-C9DB-A142-A5DA-4F726678684E}"/>
-    <hyperlink ref="G77" r:id="rId5" xr:uid="{F93640CD-F8C5-5F44-938F-F54CED5CF057}"/>
-    <hyperlink ref="G65" r:id="rId6" xr:uid="{D9E28B47-ABDD-424D-AB8F-DB2E604A9B8E}"/>
-    <hyperlink ref="G66" r:id="rId7" xr:uid="{615ECB5F-ED30-174F-9421-780B5BA01133}"/>
-    <hyperlink ref="G67" r:id="rId8" xr:uid="{641FA6F8-8360-9340-89D7-B2DD19F3D19A}"/>
-    <hyperlink ref="G68" r:id="rId9" xr:uid="{7C260904-F1A1-DE4E-93D5-151956B3864E}"/>
-    <hyperlink ref="G64" r:id="rId10" xr:uid="{0104D87D-7487-6943-AA46-BF98340F4093}"/>
-    <hyperlink ref="G69" r:id="rId11" xr:uid="{15B0D16A-8319-4E43-B560-26A6139EE942}"/>
-    <hyperlink ref="G106" r:id="rId12" xr:uid="{DB51E3FB-965C-3C44-9411-CD70840D2B69}"/>
-    <hyperlink ref="G92" r:id="rId13" xr:uid="{24AF945D-15DB-C14B-9386-9CEB06B119F7}"/>
+    <hyperlink ref="G73" r:id="rId1" xr:uid="{0A8B3BE8-26AA-754F-BFC2-92BCE65A3ED5}"/>
+    <hyperlink ref="G77" r:id="rId2" xr:uid="{3651323E-D02C-0B41-ADBD-75C73D14B3F2}"/>
+    <hyperlink ref="G79" r:id="rId3" xr:uid="{13893242-B741-7745-BC62-72A5ABF3FA62}"/>
+    <hyperlink ref="G80" r:id="rId4" xr:uid="{2960CE5E-C9DB-A142-A5DA-4F726678684E}"/>
+    <hyperlink ref="G78" r:id="rId5" xr:uid="{F93640CD-F8C5-5F44-938F-F54CED5CF057}"/>
+    <hyperlink ref="G66" r:id="rId6" xr:uid="{D9E28B47-ABDD-424D-AB8F-DB2E604A9B8E}"/>
+    <hyperlink ref="G67" r:id="rId7" xr:uid="{615ECB5F-ED30-174F-9421-780B5BA01133}"/>
+    <hyperlink ref="G68" r:id="rId8" xr:uid="{641FA6F8-8360-9340-89D7-B2DD19F3D19A}"/>
+    <hyperlink ref="G69" r:id="rId9" xr:uid="{7C260904-F1A1-DE4E-93D5-151956B3864E}"/>
+    <hyperlink ref="G65" r:id="rId10" xr:uid="{0104D87D-7487-6943-AA46-BF98340F4093}"/>
+    <hyperlink ref="G70" r:id="rId11" xr:uid="{15B0D16A-8319-4E43-B560-26A6139EE942}"/>
+    <hyperlink ref="G107" r:id="rId12" xr:uid="{DB51E3FB-965C-3C44-9411-CD70840D2B69}"/>
+    <hyperlink ref="G93" r:id="rId13" xr:uid="{24AF945D-15DB-C14B-9386-9CEB06B119F7}"/>
     <hyperlink ref="G43" r:id="rId14" xr:uid="{75952604-6765-964B-B1EA-20C7D48CD9B5}"/>
     <hyperlink ref="G42" r:id="rId15" xr:uid="{C940E895-6CF1-FB4C-9D6B-1D392B3B37A5}"/>
     <hyperlink ref="G23" r:id="rId16" xr:uid="{36F5767C-7CE9-B34E-99CD-B313F2FC62AB}"/>
@@ -5764,7 +5809,7 @@
     <hyperlink ref="G41" r:id="rId23" xr:uid="{BBE2B349-1DFD-4AA2-B438-B0588AB6D53D}"/>
     <hyperlink ref="G29" r:id="rId24" xr:uid="{2CF9A68E-9414-4C9C-90A3-DB67F15E0B77}"/>
     <hyperlink ref="G34" r:id="rId25" xr:uid="{1A7772FB-014F-49FB-BBDB-54C9FE4D8421}"/>
-    <hyperlink ref="G62" r:id="rId26" xr:uid="{BE314D45-C7EE-42A2-AD0D-BBE20F94E2F4}"/>
+    <hyperlink ref="G63" r:id="rId26" xr:uid="{BE314D45-C7EE-42A2-AD0D-BBE20F94E2F4}"/>
     <hyperlink ref="G51" r:id="rId27" xr:uid="{246EBA00-6370-4023-81D2-8AE7FA547972}"/>
     <hyperlink ref="G48" r:id="rId28" xr:uid="{9B1A161B-05C8-4CED-80A6-08C06CAC752E}"/>
     <hyperlink ref="G49" r:id="rId29" xr:uid="{5511A8B2-32B8-485B-B55B-453CB6D21F16}"/>

</xml_diff>